<commit_message>
Ajout d'opérateurs - & / Ajout de réels et retrait des entiers
</commit_message>
<xml_diff>
--- a/Table analyse.xlsx
+++ b/Table analyse.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="34">
   <si>
     <t>États</t>
   </si>
@@ -98,9 +98,6 @@
     <t>d8</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>d9</t>
   </si>
   <si>
@@ -111,23 +108,34 @@
   </si>
   <si>
     <t>r4</t>
+  </si>
+  <si>
+    <t>d10</t>
+  </si>
+  <si>
+    <t>d11</t>
+  </si>
+  <si>
+    <t>d12</t>
+  </si>
+  <si>
+    <t>d13</t>
+  </si>
+  <si>
+    <t>r6</t>
+  </si>
+  <si>
+    <t>r7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,8 +157,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,33 +207,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -287,6 +324,22 @@
         <b/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -302,20 +355,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A2:K16" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A2:K16" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
   <autoFilter ref="A2:K16"/>
   <tableColumns count="11">
-    <tableColumn id="1" name=" "/>
-    <tableColumn id="2" name="val" dataDxfId="10"/>
-    <tableColumn id="3" name="+" dataDxfId="9"/>
-    <tableColumn id="4" name="*" dataDxfId="8"/>
-    <tableColumn id="5" name="-" dataDxfId="7"/>
-    <tableColumn id="6" name="/" dataDxfId="6"/>
-    <tableColumn id="7" name="(" dataDxfId="5"/>
-    <tableColumn id="8" name=")" dataDxfId="4"/>
-    <tableColumn id="9" name="$" dataDxfId="3"/>
-    <tableColumn id="10" name="2" dataDxfId="2"/>
-    <tableColumn id="11" name="E" dataDxfId="1"/>
+    <tableColumn id="1" name=" " dataDxfId="12"/>
+    <tableColumn id="2" name="val" dataDxfId="11"/>
+    <tableColumn id="3" name="+" dataDxfId="10"/>
+    <tableColumn id="4" name="*" dataDxfId="9"/>
+    <tableColumn id="5" name="-" dataDxfId="8"/>
+    <tableColumn id="6" name="/" dataDxfId="7"/>
+    <tableColumn id="7" name="(" dataDxfId="6"/>
+    <tableColumn id="8" name=")" dataDxfId="5"/>
+    <tableColumn id="9" name="$" dataDxfId="4"/>
+    <tableColumn id="10" name="2" dataDxfId="3"/>
+    <tableColumn id="11" name="E" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -587,7 +640,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,386 +651,406 @@
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="2"/>
-      <c r="K1" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="5"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="I9" s="1"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="4"/>
+      <c r="E15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>13</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="2"/>
+      <c r="K16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:K16">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Mise à jours des diagrammes
</commit_message>
<xml_diff>
--- a/Table analyse.xlsx
+++ b/Table analyse.xlsx
@@ -234,7 +234,22 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6969"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF8B8B"/>
+          <bgColor rgb="FFFF6565"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -343,6 +358,13 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF6969"/>
+      <color rgb="FFFF6565"/>
+      <color rgb="FFFF8B8B"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -355,20 +377,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A2:K16" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A2:K16" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
   <autoFilter ref="A2:K16"/>
   <tableColumns count="11">
-    <tableColumn id="1" name=" " dataDxfId="12"/>
-    <tableColumn id="2" name="val" dataDxfId="11"/>
-    <tableColumn id="3" name="+" dataDxfId="10"/>
-    <tableColumn id="4" name="*" dataDxfId="9"/>
-    <tableColumn id="5" name="-" dataDxfId="8"/>
-    <tableColumn id="6" name="/" dataDxfId="7"/>
-    <tableColumn id="7" name="(" dataDxfId="6"/>
-    <tableColumn id="8" name=")" dataDxfId="5"/>
-    <tableColumn id="9" name="$" dataDxfId="4"/>
-    <tableColumn id="10" name="2" dataDxfId="3"/>
-    <tableColumn id="11" name="E" dataDxfId="2"/>
+    <tableColumn id="1" name=" " dataDxfId="14"/>
+    <tableColumn id="2" name="val" dataDxfId="13"/>
+    <tableColumn id="3" name="+" dataDxfId="12"/>
+    <tableColumn id="4" name="*" dataDxfId="11"/>
+    <tableColumn id="5" name="-" dataDxfId="10"/>
+    <tableColumn id="6" name="/" dataDxfId="9"/>
+    <tableColumn id="7" name="(" dataDxfId="8"/>
+    <tableColumn id="8" name=")" dataDxfId="7"/>
+    <tableColumn id="9" name="$" dataDxfId="6"/>
+    <tableColumn id="10" name="2" dataDxfId="5"/>
+    <tableColumn id="11" name="E" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -639,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,8 +1072,18 @@
     <mergeCell ref="B1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:K16">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:F16 B13:D16 G13:I16">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
+      <formula>$B$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13:K16">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout de variables définissables de manière fixe
</commit_message>
<xml_diff>
--- a/Table analyse.xlsx
+++ b/Table analyse.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
   <si>
     <t>États</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Terminaux</t>
   </si>
   <si>
-    <t>val</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
@@ -126,13 +123,25 @@
   </si>
   <si>
     <t>r7</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>reel</t>
+  </si>
+  <si>
+    <t>d14</t>
+  </si>
+  <si>
+    <t>r8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,6 +189,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -207,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -224,17 +240,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6565"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -252,15 +278,49 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF8B8B"/>
+          <bgColor rgb="FFFF6565"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -348,20 +408,22 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF6565"/>
       <color rgb="FFFF6969"/>
-      <color rgb="FFFF6565"/>
       <color rgb="FFFF8B8B"/>
     </mruColors>
   </colors>
@@ -377,20 +439,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A2:K16" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
-  <autoFilter ref="A2:K16"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name=" " dataDxfId="14"/>
-    <tableColumn id="2" name="val" dataDxfId="13"/>
-    <tableColumn id="3" name="+" dataDxfId="12"/>
-    <tableColumn id="4" name="*" dataDxfId="11"/>
-    <tableColumn id="5" name="-" dataDxfId="10"/>
-    <tableColumn id="6" name="/" dataDxfId="9"/>
-    <tableColumn id="7" name="(" dataDxfId="8"/>
-    <tableColumn id="8" name=")" dataDxfId="7"/>
-    <tableColumn id="9" name="$" dataDxfId="6"/>
-    <tableColumn id="10" name="2" dataDxfId="5"/>
-    <tableColumn id="11" name="E" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau5" displayName="Tableau5" ref="A2:L17" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A2:L17"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name=" " dataDxfId="17"/>
+    <tableColumn id="2" name="reel" dataDxfId="16"/>
+    <tableColumn id="3" name="+" dataDxfId="15"/>
+    <tableColumn id="4" name="*" dataDxfId="14"/>
+    <tableColumn id="5" name="-" dataDxfId="13"/>
+    <tableColumn id="6" name="/" dataDxfId="12"/>
+    <tableColumn id="7" name="(" dataDxfId="11"/>
+    <tableColumn id="8" name=")" dataDxfId="10"/>
+    <tableColumn id="12" name="var" dataDxfId="4"/>
+    <tableColumn id="9" name="$" dataDxfId="9"/>
+    <tableColumn id="10" name="2" dataDxfId="8"/>
+    <tableColumn id="11" name="E" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -659,431 +722,494 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="2" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="6"/>
+      <c r="L1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="1"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" s="2"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="3"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:K16">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+  <conditionalFormatting sqref="B3:H3 J3:L3 B4:L17">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:F16 B13:D16 G13:I16">
+  <conditionalFormatting sqref="E3:F17 B13:D16 G13:J16">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
+      <formula>$B$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L13:L16">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="notEqual">
       <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13:K16">
+  <conditionalFormatting sqref="I3:I17 B17:H17 J17:L17">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
-      <formula>$B$12</formula>
+      <formula>$M$6</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>